<commit_message>
included prediction time in inference method
</commit_message>
<xml_diff>
--- a/Results_benchmark/Result tables.xlsx
+++ b/Results_benchmark/Result tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guillermolambertus.v\Thesis_project_code\Results_benchmark\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BEEA5D6-5609-4508-827C-53808FB59E57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{174BB44B-83F5-4266-BBFA-836732B77803}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11670" yWindow="-21600" windowWidth="26010" windowHeight="20985" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dec 5 Model parameter tuning" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="189">
   <si>
     <t>WS parameters</t>
   </si>
@@ -666,9 +666,6 @@
     <t>Picking environment parameters FC9</t>
   </si>
   <si>
-    <t>TBD</t>
-  </si>
-  <si>
     <t>Number of scenarios (K)</t>
   </si>
   <si>
@@ -694,6 +691,285 @@
   </si>
   <si>
     <t>Objective</t>
+  </si>
+  <si>
+    <t>21/05/2025 - 27/05/2025</t>
+  </si>
+  <si>
+    <t>Model type</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>25-06-2025:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> RELIABILITY GBDT model</t>
+    </r>
+  </si>
+  <si>
+    <t>GBDT model (active frame-stacks)</t>
+  </si>
+  <si>
+    <t>GBDT model (inactive frame-stacks)</t>
+  </si>
+  <si>
+    <t>Mean baseline (inactive frame-stacks)</t>
+  </si>
+  <si>
+    <t>Deterministic model</t>
+  </si>
+  <si>
+    <t>Stochastic model</t>
+  </si>
+  <si>
+    <t>49.38</t>
+  </si>
+  <si>
+    <t>38.65</t>
+  </si>
+  <si>
+    <t>19.87</t>
+  </si>
+  <si>
+    <t>MAPE (%)</t>
+  </si>
+  <si>
+    <t>1222.62</t>
+  </si>
+  <si>
+    <t>MAE (min)</t>
+  </si>
+  <si>
+    <t>RMSE (min)</t>
+  </si>
+  <si>
+    <t>CRPS (min)</t>
+  </si>
+  <si>
+    <t>Prediction time (sec)</t>
+  </si>
+  <si>
+    <t>2438.27</t>
+  </si>
+  <si>
+    <t>46.81</t>
+  </si>
+  <si>
+    <t>35.71</t>
+  </si>
+  <si>
+    <t>18.25</t>
+  </si>
+  <si>
+    <t>2191.55</t>
+  </si>
+  <si>
+    <t>34.97</t>
+  </si>
+  <si>
+    <t>26.52</t>
+  </si>
+  <si>
+    <t>58.19</t>
+  </si>
+  <si>
+    <t>34.67</t>
+  </si>
+  <si>
+    <t>46.45</t>
+  </si>
+  <si>
+    <t>26.74</t>
+  </si>
+  <si>
+    <t>35.14</t>
+  </si>
+  <si>
+    <t>59.58</t>
+  </si>
+  <si>
+    <t>17.92</t>
+  </si>
+  <si>
+    <t>Residual variance (min^2)</t>
+  </si>
+  <si>
+    <t>2157.73</t>
+  </si>
+  <si>
+    <t>1197.35</t>
+  </si>
+  <si>
+    <t>39.76</t>
+  </si>
+  <si>
+    <t>54.76</t>
+  </si>
+  <si>
+    <t>69.25</t>
+  </si>
+  <si>
+    <t>Stochastic model implemented</t>
+  </si>
+  <si>
+    <t>Deterministic model implemented</t>
+  </si>
+  <si>
+    <t>Model implemented</t>
+  </si>
+  <si>
+    <t>Simulation type</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>25-06-2025:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> RELIABILITY GBDT model - </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>k-fold cross validation</t>
+    </r>
+  </si>
+  <si>
+    <t>Training time (sec)</t>
+  </si>
+  <si>
+    <t>14.03</t>
+  </si>
+  <si>
+    <t>0.88</t>
+  </si>
+  <si>
+    <t>53.21 ± 0.59</t>
+  </si>
+  <si>
+    <t>39.87 ± 0.18</t>
+  </si>
+  <si>
+    <t>20.24 ± 0.10</t>
+  </si>
+  <si>
+    <t>33.74 ± 0.11</t>
+  </si>
+  <si>
+    <t>24.91 ± 0.06</t>
+  </si>
+  <si>
+    <t>54.31 ± 0.27</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Results with only </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>4 shipments</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Results with only </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">4 shipments </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>benchmark</t>
+    </r>
+  </si>
+  <si>
+    <t>54.84±0.41</t>
+  </si>
+  <si>
+    <t>20.67%±0.15%</t>
+  </si>
+  <si>
+    <t>57.97±0.10</t>
+  </si>
+  <si>
+    <t>37.45±0.07</t>
+  </si>
+  <si>
+    <t>40.68±0.34</t>
+  </si>
+  <si>
+    <t>27.94±0.09</t>
+  </si>
+  <si>
+    <t>59.53%±0.26%</t>
+  </si>
+  <si>
+    <t>39.96±0.043</t>
+  </si>
+  <si>
+    <t>41.26</t>
+  </si>
+  <si>
+    <t>3911.46</t>
+  </si>
+  <si>
+    <t>Using less instances is NOT a good idea</t>
   </si>
 </sst>
 </file>
@@ -965,7 +1241,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1044,7 +1320,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1055,6 +1330,14 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1077,15 +1360,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>129428</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>74520</xdr:rowOff>
+      <xdr:colOff>453865</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>14223</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>111272</xdr:colOff>
-      <xdr:row>54</xdr:row>
-      <xdr:rowOff>35763</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>1092532</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>163245</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1108,8 +1391,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9721663" y="3652932"/>
-          <a:ext cx="9170668" cy="6498007"/>
+          <a:off x="12003394" y="5273517"/>
+          <a:ext cx="9141318" cy="6492672"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1414,26 +1697,26 @@
     <row r="2" spans="2:17" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
-      <c r="D2" s="36" t="s">
+      <c r="D2" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
-      <c r="I2" s="36"/>
-      <c r="J2" s="36" t="s">
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="36"/>
-      <c r="L2" s="36"/>
+      <c r="K2" s="35"/>
+      <c r="L2" s="35"/>
       <c r="M2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="N2" s="37" t="s">
+      <c r="N2" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="O2" s="38"/>
+      <c r="O2" s="37"/>
     </row>
     <row r="3" spans="2:17" s="1" customFormat="1" ht="20.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="4" t="s">
@@ -2227,8 +2510,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41544BC5-C3BF-460D-87C1-1B305329987F}">
   <dimension ref="B1:Q33"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2258,26 +2541,26 @@
     <row r="2" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
-      <c r="D2" s="36" t="s">
+      <c r="D2" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
-      <c r="I2" s="36"/>
-      <c r="J2" s="36" t="s">
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="36"/>
-      <c r="L2" s="36"/>
+      <c r="K2" s="35"/>
+      <c r="L2" s="35"/>
       <c r="M2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="N2" s="37" t="s">
+      <c r="N2" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="O2" s="38"/>
+      <c r="O2" s="37"/>
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
     </row>
@@ -2713,7 +2996,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="12" spans="2:17" ht="37" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:17" ht="44.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="11">
         <v>9</v>
       </c>
@@ -2764,39 +3047,95 @@
       <c r="B13" s="11">
         <v>10</v>
       </c>
-      <c r="C13" s="10"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="12"/>
-      <c r="K13" s="12"/>
-      <c r="L13" s="12"/>
-      <c r="M13" s="13"/>
-      <c r="N13" s="30"/>
-      <c r="O13" s="30"/>
-      <c r="P13" s="32"/>
+      <c r="C13" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="D13" s="12">
+        <v>38</v>
+      </c>
+      <c r="E13" s="12">
+        <v>32</v>
+      </c>
+      <c r="F13" s="12">
+        <v>16</v>
+      </c>
+      <c r="G13" s="12">
+        <v>1</v>
+      </c>
+      <c r="H13" s="12">
+        <v>8</v>
+      </c>
+      <c r="I13" s="12">
+        <v>1</v>
+      </c>
+      <c r="J13" s="12">
+        <v>3</v>
+      </c>
+      <c r="K13" s="12">
+        <v>1</v>
+      </c>
+      <c r="L13" s="12">
+        <v>2</v>
+      </c>
+      <c r="M13" s="13">
+        <v>30</v>
+      </c>
+      <c r="N13" s="30">
+        <v>1.8714999999999999</v>
+      </c>
+      <c r="O13" s="30">
+        <v>1.3746</v>
+      </c>
+      <c r="P13" s="32" t="s">
+        <v>188</v>
+      </c>
     </row>
     <row r="14" spans="2:17" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="11">
         <v>11</v>
       </c>
-      <c r="C14" s="10"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="12"/>
-      <c r="K14" s="12"/>
-      <c r="L14" s="12"/>
-      <c r="M14" s="13"/>
-      <c r="N14" s="30"/>
-      <c r="O14" s="30"/>
-      <c r="P14" s="32"/>
+      <c r="C14" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="D14" s="12">
+        <v>38</v>
+      </c>
+      <c r="E14" s="12">
+        <v>32</v>
+      </c>
+      <c r="F14" s="12">
+        <v>16</v>
+      </c>
+      <c r="G14" s="12">
+        <v>1</v>
+      </c>
+      <c r="H14" s="12">
+        <v>8</v>
+      </c>
+      <c r="I14" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="J14" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="K14" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="L14" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="M14" s="13">
+        <v>30</v>
+      </c>
+      <c r="N14" s="30">
+        <v>2.4984999999999999</v>
+      </c>
+      <c r="O14" s="30">
+        <v>1.575</v>
+      </c>
+      <c r="P14" s="32" t="s">
+        <v>188</v>
+      </c>
     </row>
     <row r="15" spans="2:17" ht="17" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="11">
@@ -3023,8 +3362,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BA4D312-E3A4-4B1B-A7BA-5A721BC68845}">
   <dimension ref="C2:I46"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3072,7 +3411,7 @@
         <v>87</v>
       </c>
       <c r="D5">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E5" t="s">
         <v>93</v>
@@ -3083,7 +3422,7 @@
         <v>107</v>
       </c>
       <c r="D6">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="E6" t="s">
         <v>93</v>
@@ -3121,7 +3460,7 @@
     </row>
     <row r="11" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D11">
         <v>70</v>
@@ -3132,7 +3471,7 @@
     </row>
     <row r="12" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D12">
         <v>2</v>
@@ -3143,7 +3482,7 @@
     </row>
     <row r="13" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D13">
         <v>3</v>
@@ -3154,7 +3493,7 @@
     </row>
     <row r="14" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C14" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -3184,7 +3523,7 @@
     </row>
     <row r="18" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C18" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D18">
         <v>70</v>
@@ -3195,7 +3534,7 @@
     </row>
     <row r="19" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C19" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D19">
         <v>2</v>
@@ -3206,7 +3545,7 @@
     </row>
     <row r="20" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C20" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D20">
         <v>3</v>
@@ -3217,7 +3556,7 @@
     </row>
     <row r="21" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C21" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -3239,7 +3578,7 @@
     </row>
     <row r="23" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C23" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E23" t="s">
         <v>93</v>
@@ -3252,10 +3591,10 @@
     </row>
     <row r="26" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C26" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D26" s="33" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E26" t="s">
         <v>93</v>
@@ -3263,10 +3602,10 @@
     </row>
     <row r="27" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C27" t="s">
-        <v>124</v>
-      </c>
-      <c r="D27" s="34" t="s">
-        <v>116</v>
+        <v>123</v>
+      </c>
+      <c r="D27" s="38" t="s">
+        <v>125</v>
       </c>
       <c r="E27" t="s">
         <v>93</v>
@@ -3276,7 +3615,7 @@
       <c r="C28" t="s">
         <v>100</v>
       </c>
-      <c r="D28" s="35">
+      <c r="D28" s="34">
         <v>5</v>
       </c>
       <c r="E28" t="s">
@@ -3309,7 +3648,7 @@
       <c r="C31" t="s">
         <v>102</v>
       </c>
-      <c r="D31" s="35" t="s">
+      <c r="D31" s="34" t="s">
         <v>95</v>
       </c>
       <c r="E31" t="s">
@@ -3367,10 +3706,10 @@
     </row>
     <row r="38" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C38" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D38" s="33" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E38" t="s">
         <v>93</v>
@@ -3378,10 +3717,10 @@
     </row>
     <row r="39" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C39" t="s">
-        <v>124</v>
-      </c>
-      <c r="D39" s="34" t="s">
-        <v>116</v>
+        <v>123</v>
+      </c>
+      <c r="D39" s="38" t="s">
+        <v>125</v>
       </c>
       <c r="E39" t="s">
         <v>93</v>
@@ -3391,7 +3730,7 @@
       <c r="C40" t="s">
         <v>100</v>
       </c>
-      <c r="D40" s="35">
+      <c r="D40" s="34">
         <v>5</v>
       </c>
       <c r="E40" t="s">
@@ -3424,7 +3763,7 @@
       <c r="C43" t="s">
         <v>102</v>
       </c>
-      <c r="D43" s="35" t="s">
+      <c r="D43" s="34" t="s">
         <v>95</v>
       </c>
       <c r="E43" t="s">
@@ -3471,26 +3810,42 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B4CCA38-C1E8-4E87-B1AA-966A071EE4EA}">
-  <dimension ref="B2:E15"/>
+  <dimension ref="B2:U35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E15" sqref="B9:E15"/>
+    <sheetView topLeftCell="E1" zoomScale="114" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S22" sqref="S22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="30.453125" customWidth="1"/>
     <col min="3" max="3" width="23.36328125" customWidth="1"/>
-    <col min="4" max="4" width="24.81640625" customWidth="1"/>
-    <col min="5" max="5" width="23.6328125" customWidth="1"/>
+    <col min="4" max="4" width="32.90625" customWidth="1"/>
+    <col min="5" max="5" width="25" customWidth="1"/>
+    <col min="6" max="6" width="24.7265625" customWidth="1"/>
+    <col min="7" max="7" width="13.36328125" customWidth="1"/>
+    <col min="8" max="8" width="34" customWidth="1"/>
+    <col min="9" max="9" width="10.81640625" customWidth="1"/>
+    <col min="10" max="10" width="11" customWidth="1"/>
+    <col min="11" max="11" width="22.81640625" customWidth="1"/>
+    <col min="12" max="12" width="12.54296875" customWidth="1"/>
+    <col min="13" max="13" width="18" customWidth="1"/>
+    <col min="14" max="14" width="20.7265625" customWidth="1"/>
+    <col min="15" max="15" width="18.453125" customWidth="1"/>
+    <col min="16" max="16" width="7.453125" customWidth="1"/>
+    <col min="17" max="17" width="32.26953125" customWidth="1"/>
+    <col min="18" max="18" width="11.7265625" customWidth="1"/>
+    <col min="19" max="19" width="12.26953125" customWidth="1"/>
+    <col min="20" max="20" width="12.54296875" customWidth="1"/>
+    <col min="21" max="21" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="22" t="s">
         <v>49</v>
       </c>
@@ -3504,9 +3859,9 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="2:5" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:21" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B4" s="20" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C4" s="21">
         <v>-0.48249999999999998</v>
@@ -3518,7 +3873,7 @@
         <v>3.782</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B5" s="20" t="s">
         <v>53</v>
       </c>
@@ -3532,7 +3887,7 @@
         <v>149.77000000000001</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B6" s="20" t="s">
         <v>54</v>
       </c>
@@ -3546,7 +3901,7 @@
         <v>1332</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B7" s="20" t="s">
         <v>55</v>
       </c>
@@ -3560,80 +3915,506 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="11" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H10" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="11" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B11" s="22" t="s">
+        <v>165</v>
+      </c>
+      <c r="C11" s="23" t="s">
+        <v>124</v>
+      </c>
+      <c r="D11" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="E11" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="F11" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="H11" s="22" t="s">
+        <v>126</v>
+      </c>
+      <c r="I11" s="23" t="s">
+        <v>139</v>
+      </c>
+      <c r="J11" s="23" t="s">
+        <v>138</v>
+      </c>
+      <c r="K11" s="23" t="s">
+        <v>136</v>
+      </c>
+      <c r="L11" s="23" t="s">
+        <v>156</v>
+      </c>
+      <c r="M11" s="23" t="s">
+        <v>140</v>
+      </c>
+      <c r="N11" s="23" t="s">
+        <v>167</v>
+      </c>
+      <c r="O11" s="23" t="s">
+        <v>141</v>
+      </c>
+      <c r="Q11" s="22" t="s">
+        <v>126</v>
+      </c>
+      <c r="R11" s="23" t="s">
+        <v>139</v>
+      </c>
+      <c r="S11" s="23" t="s">
+        <v>138</v>
+      </c>
+      <c r="T11" s="23" t="s">
+        <v>136</v>
+      </c>
+      <c r="U11" s="23" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="12" spans="2:21" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="45" t="s">
+        <v>163</v>
+      </c>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="21"/>
+      <c r="H12" s="41" t="s">
+        <v>131</v>
+      </c>
+      <c r="I12" s="21"/>
+      <c r="J12" s="21"/>
+      <c r="K12" s="21"/>
+      <c r="L12" s="21"/>
+      <c r="M12" s="21"/>
+      <c r="N12" s="21"/>
+      <c r="O12" s="21"/>
+      <c r="Q12" s="41" t="s">
+        <v>131</v>
+      </c>
+      <c r="S12" s="21"/>
+      <c r="T12" s="21"/>
+      <c r="U12" s="21"/>
+    </row>
+    <row r="13" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="B13" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13" s="44">
+        <v>-3959</v>
+      </c>
+      <c r="D13" s="21">
+        <v>207.6</v>
+      </c>
+      <c r="E13" s="21">
+        <v>1525</v>
+      </c>
+      <c r="F13" s="21">
+        <v>62</v>
+      </c>
+      <c r="H13" s="20" t="s">
+        <v>128</v>
+      </c>
+      <c r="I13" s="21" t="s">
+        <v>147</v>
+      </c>
+      <c r="J13" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="K13" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="L13" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="M13" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="N13" s="21" t="s">
+        <v>168</v>
+      </c>
+      <c r="O13" s="21"/>
+      <c r="Q13" s="20" t="s">
+        <v>128</v>
+      </c>
+      <c r="R13" t="s">
+        <v>173</v>
+      </c>
+      <c r="S13" s="21" t="s">
+        <v>174</v>
+      </c>
+      <c r="T13" s="21" t="s">
+        <v>175</v>
+      </c>
+      <c r="U13" s="21" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="14" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="B14" s="20" t="s">
+        <v>164</v>
+      </c>
+      <c r="C14" s="21">
+        <v>-0.85550000000000004</v>
+      </c>
+      <c r="D14" s="21">
+        <v>197.2</v>
+      </c>
+      <c r="E14" s="21">
+        <v>1029</v>
+      </c>
+      <c r="F14" s="21">
         <v>49</v>
       </c>
-      <c r="C11" s="23" t="s">
+      <c r="H14" s="20" t="s">
+        <v>129</v>
+      </c>
+      <c r="I14" s="21" t="s">
+        <v>143</v>
+      </c>
+      <c r="J14" s="21" t="s">
+        <v>144</v>
+      </c>
+      <c r="K14" s="21" t="s">
+        <v>145</v>
+      </c>
+      <c r="L14" s="21" t="s">
+        <v>146</v>
+      </c>
+      <c r="M14" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="N14" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="O14" s="21"/>
+      <c r="Q14" s="20" t="s">
+        <v>129</v>
+      </c>
+      <c r="R14" s="21" t="s">
+        <v>170</v>
+      </c>
+      <c r="S14" s="21" t="s">
+        <v>171</v>
+      </c>
+      <c r="T14" s="21" t="s">
+        <v>172</v>
+      </c>
+      <c r="U14" s="21" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="15" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="B15" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" s="21">
+        <v>12.52</v>
+      </c>
+      <c r="D15" s="21">
+        <v>202.5</v>
+      </c>
+      <c r="E15" s="21">
+        <v>320</v>
+      </c>
+      <c r="F15" s="21">
+        <v>15</v>
+      </c>
+      <c r="H15" s="39" t="s">
+        <v>130</v>
+      </c>
+      <c r="I15" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="J15" s="21" t="s">
+        <v>134</v>
+      </c>
+      <c r="K15" s="21" t="s">
+        <v>135</v>
+      </c>
+      <c r="L15" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="M15" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="N15" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="O15" s="21"/>
+      <c r="Q15" s="39"/>
+      <c r="R15" s="21"/>
+      <c r="S15" s="21"/>
+      <c r="T15" s="21"/>
+      <c r="U15" s="21"/>
+    </row>
+    <row r="16" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="B16" s="20"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="21"/>
+      <c r="H16" s="42"/>
+      <c r="I16" s="21"/>
+      <c r="J16" s="21"/>
+      <c r="K16" s="21"/>
+      <c r="L16" s="21"/>
+      <c r="M16" s="21"/>
+      <c r="N16" s="21"/>
+      <c r="O16" s="21"/>
+      <c r="Q16" s="41" t="s">
+        <v>132</v>
+      </c>
+      <c r="R16" s="21"/>
+      <c r="S16" s="21"/>
+      <c r="T16" s="21"/>
+      <c r="U16" s="21"/>
+    </row>
+    <row r="17" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="B17" s="45" t="s">
+        <v>162</v>
+      </c>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="21"/>
+      <c r="H17" s="41" t="s">
+        <v>132</v>
+      </c>
+      <c r="I17" s="21"/>
+      <c r="J17" s="21"/>
+      <c r="K17" s="21"/>
+      <c r="L17" s="21"/>
+      <c r="M17" s="21"/>
+      <c r="N17" s="21"/>
+      <c r="O17" s="21"/>
+      <c r="Q17" s="20" t="s">
+        <v>128</v>
+      </c>
+      <c r="R17" s="21" t="s">
+        <v>181</v>
+      </c>
+      <c r="S17" s="21" t="s">
+        <v>183</v>
+      </c>
+      <c r="T17" s="21" t="s">
+        <v>184</v>
+      </c>
+      <c r="U17" s="21" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="18" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="B18" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="D11" s="23" t="s">
-        <v>51</v>
-      </c>
-      <c r="E11" s="24" t="s">
+      <c r="C18" s="44">
+        <v>-3959</v>
+      </c>
+      <c r="D18" s="21">
+        <v>207.6</v>
+      </c>
+      <c r="E18" s="21">
+        <v>1525</v>
+      </c>
+      <c r="F18" s="21">
+        <v>62</v>
+      </c>
+      <c r="H18" s="20" t="s">
+        <v>128</v>
+      </c>
+      <c r="I18" s="21" t="s">
+        <v>150</v>
+      </c>
+      <c r="J18" s="21" t="s">
+        <v>152</v>
+      </c>
+      <c r="K18" s="21" t="s">
+        <v>154</v>
+      </c>
+      <c r="L18" s="21" t="s">
+        <v>158</v>
+      </c>
+      <c r="M18" s="44" t="s">
+        <v>159</v>
+      </c>
+      <c r="N18" s="21" t="s">
+        <v>187</v>
+      </c>
+      <c r="O18" s="21"/>
+      <c r="Q18" s="20" t="s">
+        <v>129</v>
+      </c>
+      <c r="R18" s="21" t="s">
+        <v>178</v>
+      </c>
+      <c r="S18" s="21" t="s">
+        <v>182</v>
+      </c>
+      <c r="T18" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="U18" s="21" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="19" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="B19" s="20" t="s">
+        <v>164</v>
+      </c>
+      <c r="C19" s="21"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="21"/>
+      <c r="H19" s="20" t="s">
+        <v>129</v>
+      </c>
+      <c r="I19" s="21" t="s">
+        <v>151</v>
+      </c>
+      <c r="J19" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="K19" s="21" t="s">
+        <v>155</v>
+      </c>
+      <c r="L19" s="21" t="s">
+        <v>157</v>
+      </c>
+      <c r="M19" s="21" t="s">
+        <v>160</v>
+      </c>
+      <c r="N19" s="21" t="s">
+        <v>186</v>
+      </c>
+      <c r="O19" s="21"/>
+      <c r="P19" s="40"/>
+      <c r="Q19" s="40"/>
+      <c r="R19" s="40"/>
+      <c r="S19" s="40"/>
+      <c r="T19" s="40"/>
+    </row>
+    <row r="20" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="B20" s="20" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="12" spans="2:5" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="20" t="s">
-        <v>125</v>
-      </c>
-      <c r="C12" s="21">
-        <v>-3.9590000000000001</v>
-      </c>
-      <c r="D12" s="21">
-        <v>-0.85550000000000004</v>
-      </c>
-      <c r="E12">
-        <v>12.52</v>
-      </c>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B13" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="C13" s="21">
-        <v>207.55</v>
-      </c>
-      <c r="D13" s="21">
-        <v>197.2</v>
-      </c>
-      <c r="E13">
-        <v>202.5</v>
-      </c>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B14" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="C14" s="21">
-        <v>1525</v>
-      </c>
-      <c r="D14" s="21">
-        <v>1029</v>
-      </c>
-      <c r="E14">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B15" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="C15" s="21">
-        <v>62</v>
-      </c>
-      <c r="D15" s="21">
-        <v>49</v>
-      </c>
-      <c r="E15">
-        <v>15</v>
-      </c>
+      <c r="C20" s="21"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="21"/>
+      <c r="H20" s="39" t="s">
+        <v>130</v>
+      </c>
+      <c r="I20" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="J20" s="21" t="s">
+        <v>134</v>
+      </c>
+      <c r="K20" s="21" t="s">
+        <v>135</v>
+      </c>
+      <c r="L20" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="M20" s="21" t="s">
+        <v>161</v>
+      </c>
+      <c r="N20" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="O20" s="21"/>
+      <c r="P20" s="40"/>
+      <c r="Q20" s="40"/>
+      <c r="R20" s="40"/>
+      <c r="S20" s="40"/>
+      <c r="T20" s="40"/>
+    </row>
+    <row r="21" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="B21" s="40"/>
+      <c r="C21" s="40"/>
+      <c r="D21" s="40"/>
+      <c r="E21" s="40"/>
+      <c r="H21" s="43"/>
+      <c r="I21" s="40"/>
+      <c r="J21" s="40"/>
+      <c r="K21" s="40"/>
+      <c r="L21" s="40"/>
+      <c r="M21" s="40"/>
+      <c r="N21" s="40"/>
+      <c r="O21" s="40"/>
+      <c r="P21" s="40"/>
+      <c r="Q21" s="40"/>
+      <c r="R21" s="40"/>
+      <c r="S21" s="40"/>
+      <c r="T21" s="40"/>
+    </row>
+    <row r="22" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="B22" s="40"/>
+      <c r="C22" s="40"/>
+      <c r="D22" s="40"/>
+      <c r="E22" s="40"/>
+      <c r="G22" s="40"/>
+      <c r="H22" s="40"/>
+      <c r="I22" s="40"/>
+      <c r="J22" s="40"/>
+      <c r="K22" s="40"/>
+      <c r="L22" s="40"/>
+      <c r="M22" s="40"/>
+      <c r="N22" s="40"/>
+      <c r="O22" s="40"/>
+      <c r="P22" s="40"/>
+      <c r="Q22" s="40"/>
+    </row>
+    <row r="23" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="B23" s="40"/>
+      <c r="C23" s="40"/>
+      <c r="D23" s="40"/>
+      <c r="E23" s="40"/>
+      <c r="G23" s="39"/>
+      <c r="H23" s="40"/>
+      <c r="I23" s="40"/>
+      <c r="J23" s="40"/>
+      <c r="K23" s="40"/>
+      <c r="L23" s="40"/>
+      <c r="M23" s="40"/>
+      <c r="N23" s="40"/>
+      <c r="O23" s="40"/>
+    </row>
+    <row r="24" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="D24" s="40"/>
+      <c r="E24" s="40"/>
+      <c r="G24" s="40"/>
+      <c r="I24" s="40"/>
+      <c r="L24" s="40"/>
+      <c r="M24" s="40"/>
+      <c r="N24" s="40"/>
+    </row>
+    <row r="25" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="D25" s="40"/>
+      <c r="N25" s="40"/>
+    </row>
+    <row r="26" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="D26" s="40"/>
+      <c r="N26" s="40"/>
+    </row>
+    <row r="27" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="D27" s="40"/>
+    </row>
+    <row r="35" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="E35" s="40"/>
+      <c r="F35" s="40"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Changed visualization of confidence intervals to make it correct
</commit_message>
<xml_diff>
--- a/Results_benchmark/Result tables.xlsx
+++ b/Results_benchmark/Result tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guillermolambertus.v\Thesis_project_code\Results_benchmark\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A15BAE6-CF7E-4185-A893-E90CF23362F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A0FAEFF-60DE-43CD-8F28-C7ED6E6576CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14145" yWindow="-21720" windowWidth="51840" windowHeight="21120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-30" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Det param tuning 5 Dec" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="226">
   <si>
     <t>WS parameters</t>
   </si>
@@ -969,6 +969,43 @@
   </si>
   <si>
     <t>Reduce period for trigger to 12</t>
+  </si>
+  <si>
+    <t>Performance slightly better, but not as good as the deterministic model with 3 minutes</t>
+  </si>
+  <si>
+    <t>Periodic trigger at 12 minutes instead of 3</t>
+  </si>
+  <si>
+    <t>Not good compared to periodic trigger of 3 min</t>
+  </si>
+  <si>
+    <t>Reduce period for trigger to 6</t>
+  </si>
+  <si>
+    <t>Periodic trigger at 6 minutes instead of 3</t>
+  </si>
+  <si>
+    <t>Optimality getting better when decreasing trigger period</t>
+  </si>
+  <si>
+    <t>Optimality keeps on getting better when increasing trigger frequency</t>
+  </si>
+  <si>
+    <t>Reduce period for trigger to 3</t>
+  </si>
+  <si>
+    <t>Optimality is now even better</t>
+  </si>
+  <si>
+    <t>Optimality suddenly worse</t>
+  </si>
+  <si>
+    <t>Periodic trigger at 3, to obtain deterministic
+reliability metrics</t>
+  </si>
+  <si>
+    <t>Increase scenario count to 5</t>
   </si>
 </sst>
 </file>
@@ -1371,7 +1408,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1453,6 +1490,33 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1462,18 +1526,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1483,26 +1535,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1923,26 +1956,26 @@
     <row r="2" spans="2:17" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
-      <c r="D2" s="37" t="s">
+      <c r="D2" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37" t="s">
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="52"/>
+      <c r="J2" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="37"/>
-      <c r="L2" s="37"/>
+      <c r="K2" s="52"/>
+      <c r="L2" s="52"/>
       <c r="M2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="N2" s="38" t="s">
+      <c r="N2" s="53" t="s">
         <v>15</v>
       </c>
-      <c r="O2" s="39"/>
+      <c r="O2" s="54"/>
     </row>
     <row r="3" spans="2:17" s="1" customFormat="1" ht="20.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="4" t="s">
@@ -2736,13 +2769,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41544BC5-C3BF-460D-87C1-1B305329987F}">
   <dimension ref="B1:Q33"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F40" sqref="F40"/>
+    <sheetView topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="42.36328125" customWidth="1"/>
+    <col min="3" max="3" width="43.7265625" customWidth="1"/>
     <col min="4" max="4" width="19.54296875" customWidth="1"/>
     <col min="5" max="5" width="22" customWidth="1"/>
     <col min="6" max="6" width="26.26953125" customWidth="1"/>
@@ -2755,7 +2788,7 @@
     <col min="13" max="13" width="32.81640625" customWidth="1"/>
     <col min="14" max="14" width="45.54296875" customWidth="1"/>
     <col min="15" max="15" width="33" customWidth="1"/>
-    <col min="16" max="16" width="49.7265625" customWidth="1"/>
+    <col min="16" max="16" width="54.26953125" customWidth="1"/>
     <col min="17" max="17" width="15.54296875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2767,26 +2800,26 @@
     <row r="2" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
-      <c r="D2" s="37" t="s">
+      <c r="D2" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37" t="s">
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="52"/>
+      <c r="J2" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="37"/>
-      <c r="L2" s="37"/>
+      <c r="K2" s="52"/>
+      <c r="L2" s="52"/>
       <c r="M2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="N2" s="38" t="s">
+      <c r="N2" s="53" t="s">
         <v>15</v>
       </c>
-      <c r="O2" s="39"/>
+      <c r="O2" s="54"/>
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
     </row>
@@ -3363,62 +3396,146 @@
         <v>180</v>
       </c>
     </row>
-    <row r="15" spans="2:17" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:17" ht="32" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="11">
         <v>12</v>
       </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="12"/>
-      <c r="J15" s="12"/>
-      <c r="K15" s="12"/>
-      <c r="L15" s="12"/>
-      <c r="M15" s="13"/>
-      <c r="N15" s="30"/>
-      <c r="O15" s="30"/>
-      <c r="P15" s="32"/>
-    </row>
-    <row r="16" spans="2:17" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C15" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="D15" s="12">
+        <v>38</v>
+      </c>
+      <c r="E15" s="12">
+        <v>32</v>
+      </c>
+      <c r="F15" s="12">
+        <v>16</v>
+      </c>
+      <c r="G15" s="12">
+        <v>1</v>
+      </c>
+      <c r="H15" s="12">
+        <v>8</v>
+      </c>
+      <c r="I15" s="12">
+        <v>1</v>
+      </c>
+      <c r="J15" s="12">
+        <v>12</v>
+      </c>
+      <c r="K15" s="12">
+        <v>1</v>
+      </c>
+      <c r="L15" s="12">
+        <v>2</v>
+      </c>
+      <c r="M15" s="13">
+        <v>30</v>
+      </c>
+      <c r="N15" s="30">
+        <v>-3.5154000000000001</v>
+      </c>
+      <c r="O15" s="30">
+        <v>8.7833000000000006</v>
+      </c>
+      <c r="P15" s="32" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="16" spans="2:17" ht="32" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="11">
         <v>13</v>
       </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="12"/>
-      <c r="J16" s="12"/>
-      <c r="K16" s="12"/>
-      <c r="L16" s="12"/>
-      <c r="M16" s="13"/>
-      <c r="N16" s="30"/>
-      <c r="O16" s="30"/>
-      <c r="P16" s="32"/>
-    </row>
-    <row r="17" spans="2:16" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C16" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="D16" s="12">
+        <v>38</v>
+      </c>
+      <c r="E16" s="12">
+        <v>32</v>
+      </c>
+      <c r="F16" s="12">
+        <v>16</v>
+      </c>
+      <c r="G16" s="12">
+        <v>1</v>
+      </c>
+      <c r="H16" s="12">
+        <v>8</v>
+      </c>
+      <c r="I16" s="12">
+        <v>1</v>
+      </c>
+      <c r="J16" s="12">
+        <v>6</v>
+      </c>
+      <c r="K16" s="12">
+        <v>1</v>
+      </c>
+      <c r="L16" s="12">
+        <v>2</v>
+      </c>
+      <c r="M16" s="13">
+        <v>30</v>
+      </c>
+      <c r="N16" s="30">
+        <v>-1.387</v>
+      </c>
+      <c r="O16" s="30">
+        <v>12.126200000000001</v>
+      </c>
+      <c r="P16" s="32" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="17" spans="2:16" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" s="11">
         <v>14</v>
       </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="12"/>
-      <c r="J17" s="12"/>
-      <c r="K17" s="12"/>
-      <c r="L17" s="12"/>
-      <c r="M17" s="13"/>
-      <c r="N17" s="30"/>
-      <c r="O17" s="30"/>
-      <c r="P17" s="32"/>
+      <c r="C17" s="10" t="s">
+        <v>224</v>
+      </c>
+      <c r="D17" s="12">
+        <v>38</v>
+      </c>
+      <c r="E17" s="12">
+        <v>32</v>
+      </c>
+      <c r="F17" s="12">
+        <v>16</v>
+      </c>
+      <c r="G17" s="12">
+        <v>1</v>
+      </c>
+      <c r="H17" s="12">
+        <v>8</v>
+      </c>
+      <c r="I17" s="12">
+        <v>1</v>
+      </c>
+      <c r="J17" s="12">
+        <v>3</v>
+      </c>
+      <c r="K17" s="12">
+        <v>1</v>
+      </c>
+      <c r="L17" s="12">
+        <v>2</v>
+      </c>
+      <c r="M17" s="13">
+        <v>30</v>
+      </c>
+      <c r="N17" s="30">
+        <v>-3.2052</v>
+      </c>
+      <c r="O17" s="30">
+        <v>9.6207999999999991</v>
+      </c>
+      <c r="P17" s="58" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="18" spans="2:16" ht="17" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B18" s="11">
@@ -3588,8 +3705,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F60761B3-7DE1-4115-A7F0-B8A9476CC7B3}">
   <dimension ref="B1:S33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3603,7 +3720,8 @@
     <col min="15" max="15" width="31.90625" customWidth="1"/>
     <col min="16" max="16" width="34.7265625" customWidth="1"/>
     <col min="17" max="17" width="22.54296875" customWidth="1"/>
-    <col min="18" max="18" width="28.26953125" customWidth="1"/>
+    <col min="18" max="18" width="32.90625" customWidth="1"/>
+    <col min="19" max="19" width="11.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:19" ht="32.5" thickBot="1" x14ac:dyDescent="0.75">
@@ -3614,28 +3732,28 @@
     <row r="2" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
-      <c r="D2" s="37" t="s">
+      <c r="D2" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37" t="s">
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="52"/>
+      <c r="J2" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="37"/>
-      <c r="L2" s="37"/>
-      <c r="M2" s="37"/>
-      <c r="N2" s="37"/>
+      <c r="K2" s="52"/>
+      <c r="L2" s="52"/>
+      <c r="M2" s="52"/>
+      <c r="N2" s="52"/>
       <c r="O2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="P2" s="38" t="s">
+      <c r="P2" s="53" t="s">
         <v>15</v>
       </c>
-      <c r="Q2" s="39"/>
+      <c r="Q2" s="54"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
     </row>
@@ -3682,10 +3800,10 @@
       <c r="O3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="P3" s="40" t="s">
+      <c r="P3" s="37" t="s">
         <v>191</v>
       </c>
-      <c r="Q3" s="41" t="s">
+      <c r="Q3" s="38" t="s">
         <v>192</v>
       </c>
       <c r="R3" s="26" t="s">
@@ -3803,7 +3921,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="6" spans="2:19" ht="33" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:19" ht="47" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="11">
         <v>3</v>
       </c>
@@ -3846,69 +3964,168 @@
       <c r="O6" s="13">
         <v>30</v>
       </c>
-      <c r="P6" s="30"/>
-      <c r="Q6" s="30"/>
-      <c r="R6" s="31"/>
+      <c r="P6" s="30">
+        <v>-3.1383000000000001</v>
+      </c>
+      <c r="Q6" s="30">
+        <v>10.653700000000001</v>
+      </c>
+      <c r="R6" s="31" t="s">
+        <v>214</v>
+      </c>
     </row>
     <row r="7" spans="2:19" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" s="11">
         <v>4</v>
       </c>
-      <c r="C7" s="10"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
-      <c r="K7" s="12"/>
-      <c r="L7" s="12"/>
-      <c r="M7" s="12"/>
-      <c r="N7" s="12"/>
-      <c r="O7" s="13"/>
-      <c r="P7" s="30"/>
-      <c r="Q7" s="30"/>
-      <c r="R7" s="31"/>
+      <c r="C7" s="10" t="s">
+        <v>217</v>
+      </c>
+      <c r="D7" s="12">
+        <v>38</v>
+      </c>
+      <c r="E7" s="12">
+        <v>32</v>
+      </c>
+      <c r="F7" s="12">
+        <v>16</v>
+      </c>
+      <c r="G7" s="12">
+        <v>1</v>
+      </c>
+      <c r="H7" s="12">
+        <v>8</v>
+      </c>
+      <c r="I7" s="12">
+        <v>1</v>
+      </c>
+      <c r="J7" s="12">
+        <v>6</v>
+      </c>
+      <c r="K7" s="12">
+        <v>1</v>
+      </c>
+      <c r="L7" s="12">
+        <v>2</v>
+      </c>
+      <c r="M7" s="12">
+        <v>3</v>
+      </c>
+      <c r="N7" s="12">
+        <v>1</v>
+      </c>
+      <c r="O7" s="13">
+        <v>30</v>
+      </c>
+      <c r="P7" s="30">
+        <v>-2.4828999999999999</v>
+      </c>
+      <c r="Q7" s="30">
+        <v>11.2143</v>
+      </c>
+      <c r="R7" s="31" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="8" spans="2:19" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="11">
         <v>5</v>
       </c>
-      <c r="C8" s="10"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="12"/>
-      <c r="K8" s="12"/>
-      <c r="L8" s="12"/>
-      <c r="M8" s="12"/>
-      <c r="N8" s="12"/>
-      <c r="O8" s="13"/>
-      <c r="P8" s="30"/>
-      <c r="Q8" s="30"/>
-      <c r="R8" s="32"/>
+      <c r="C8" s="10" t="s">
+        <v>221</v>
+      </c>
+      <c r="D8" s="12">
+        <v>38</v>
+      </c>
+      <c r="E8" s="12">
+        <v>32</v>
+      </c>
+      <c r="F8" s="12">
+        <v>16</v>
+      </c>
+      <c r="G8" s="12">
+        <v>1</v>
+      </c>
+      <c r="H8" s="12">
+        <v>8</v>
+      </c>
+      <c r="I8" s="12">
+        <v>1</v>
+      </c>
+      <c r="J8" s="12">
+        <v>3</v>
+      </c>
+      <c r="K8" s="12">
+        <v>1</v>
+      </c>
+      <c r="L8" s="12">
+        <v>2</v>
+      </c>
+      <c r="M8" s="12">
+        <v>3</v>
+      </c>
+      <c r="N8" s="12">
+        <v>1</v>
+      </c>
+      <c r="O8" s="13">
+        <v>30</v>
+      </c>
+      <c r="P8" s="30">
+        <v>-1.4529000000000001</v>
+      </c>
+      <c r="Q8" s="30">
+        <v>11.4998</v>
+      </c>
+      <c r="R8" s="32" t="s">
+        <v>222</v>
+      </c>
+      <c r="S8" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="9" spans="2:19" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="11">
         <v>6</v>
       </c>
-      <c r="C9" s="10"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="12"/>
-      <c r="K9" s="12"/>
-      <c r="L9" s="12"/>
-      <c r="M9" s="12"/>
-      <c r="N9" s="12"/>
-      <c r="O9" s="13"/>
+      <c r="C9" s="10" t="s">
+        <v>225</v>
+      </c>
+      <c r="D9" s="12">
+        <v>38</v>
+      </c>
+      <c r="E9" s="12">
+        <v>32</v>
+      </c>
+      <c r="F9" s="12">
+        <v>16</v>
+      </c>
+      <c r="G9" s="12">
+        <v>1</v>
+      </c>
+      <c r="H9" s="12">
+        <v>8</v>
+      </c>
+      <c r="I9" s="12">
+        <v>1</v>
+      </c>
+      <c r="J9" s="12">
+        <v>3</v>
+      </c>
+      <c r="K9" s="12">
+        <v>1</v>
+      </c>
+      <c r="L9" s="12">
+        <v>2</v>
+      </c>
+      <c r="M9" s="12">
+        <v>4</v>
+      </c>
+      <c r="N9" s="12">
+        <v>1</v>
+      </c>
+      <c r="O9" s="13">
+        <v>30</v>
+      </c>
       <c r="P9" s="30"/>
       <c r="Q9" s="30"/>
       <c r="R9" s="31"/>
@@ -4293,230 +4510,230 @@
       <c r="B3" s="24" t="s">
         <v>160</v>
       </c>
-      <c r="C3" s="48" t="s">
+      <c r="C3" s="55" t="s">
         <v>120</v>
       </c>
-      <c r="D3" s="49"/>
-      <c r="E3" s="49"/>
-      <c r="F3" s="49"/>
-      <c r="G3" s="49"/>
-      <c r="H3" s="49"/>
-      <c r="I3" s="49"/>
-      <c r="J3" s="49"/>
-      <c r="K3" s="49"/>
-      <c r="L3" s="50"/>
-      <c r="M3" s="48" t="s">
+      <c r="D3" s="56"/>
+      <c r="E3" s="56"/>
+      <c r="F3" s="56"/>
+      <c r="G3" s="56"/>
+      <c r="H3" s="56"/>
+      <c r="I3" s="56"/>
+      <c r="J3" s="56"/>
+      <c r="K3" s="56"/>
+      <c r="L3" s="57"/>
+      <c r="M3" s="55" t="s">
         <v>51</v>
       </c>
-      <c r="N3" s="49"/>
-      <c r="O3" s="49"/>
-      <c r="P3" s="49"/>
-      <c r="Q3" s="49"/>
-      <c r="R3" s="49"/>
-      <c r="S3" s="49"/>
-      <c r="T3" s="49"/>
-      <c r="U3" s="49"/>
-      <c r="V3" s="50"/>
-      <c r="W3" s="48" t="s">
+      <c r="N3" s="56"/>
+      <c r="O3" s="56"/>
+      <c r="P3" s="56"/>
+      <c r="Q3" s="56"/>
+      <c r="R3" s="56"/>
+      <c r="S3" s="56"/>
+      <c r="T3" s="56"/>
+      <c r="U3" s="56"/>
+      <c r="V3" s="57"/>
+      <c r="W3" s="55" t="s">
         <v>52</v>
       </c>
-      <c r="X3" s="49"/>
-      <c r="Y3" s="49"/>
-      <c r="Z3" s="49"/>
-      <c r="AA3" s="49"/>
-      <c r="AB3" s="49"/>
-      <c r="AC3" s="49"/>
-      <c r="AD3" s="49"/>
-      <c r="AE3" s="49"/>
-      <c r="AF3" s="50"/>
-      <c r="AG3" s="48" t="s">
+      <c r="X3" s="56"/>
+      <c r="Y3" s="56"/>
+      <c r="Z3" s="56"/>
+      <c r="AA3" s="56"/>
+      <c r="AB3" s="56"/>
+      <c r="AC3" s="56"/>
+      <c r="AD3" s="56"/>
+      <c r="AE3" s="56"/>
+      <c r="AF3" s="57"/>
+      <c r="AG3" s="55" t="s">
         <v>53</v>
       </c>
-      <c r="AH3" s="49"/>
-      <c r="AI3" s="49"/>
-      <c r="AJ3" s="49"/>
-      <c r="AK3" s="49"/>
-      <c r="AL3" s="49"/>
-      <c r="AM3" s="49"/>
-      <c r="AN3" s="49"/>
-      <c r="AO3" s="49"/>
-      <c r="AP3" s="50"/>
-    </row>
-    <row r="4" spans="2:42" s="47" customFormat="1" ht="23" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="62" t="s">
+      <c r="AH3" s="56"/>
+      <c r="AI3" s="56"/>
+      <c r="AJ3" s="56"/>
+      <c r="AK3" s="56"/>
+      <c r="AL3" s="56"/>
+      <c r="AM3" s="56"/>
+      <c r="AN3" s="56"/>
+      <c r="AO3" s="56"/>
+      <c r="AP3" s="57"/>
+    </row>
+    <row r="4" spans="2:42" ht="23" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="51" t="s">
         <v>209</v>
       </c>
-      <c r="C4" s="59" t="s">
+      <c r="C4" s="48" t="s">
         <v>199</v>
       </c>
-      <c r="D4" s="60" t="s">
+      <c r="D4" s="49" t="s">
         <v>200</v>
       </c>
-      <c r="E4" s="59" t="s">
+      <c r="E4" s="48" t="s">
         <v>201</v>
       </c>
-      <c r="F4" s="59" t="s">
+      <c r="F4" s="48" t="s">
         <v>202</v>
       </c>
-      <c r="G4" s="60" t="s">
+      <c r="G4" s="49" t="s">
         <v>203</v>
       </c>
-      <c r="H4" s="59" t="s">
+      <c r="H4" s="48" t="s">
         <v>204</v>
       </c>
-      <c r="I4" s="59" t="s">
+      <c r="I4" s="48" t="s">
         <v>205</v>
       </c>
-      <c r="J4" s="60" t="s">
+      <c r="J4" s="49" t="s">
         <v>206</v>
       </c>
-      <c r="K4" s="59" t="s">
+      <c r="K4" s="48" t="s">
         <v>207</v>
       </c>
-      <c r="L4" s="61" t="s">
+      <c r="L4" s="50" t="s">
         <v>208</v>
       </c>
-      <c r="M4" s="59" t="s">
+      <c r="M4" s="48" t="s">
         <v>199</v>
       </c>
-      <c r="N4" s="60" t="s">
+      <c r="N4" s="49" t="s">
         <v>200</v>
       </c>
-      <c r="O4" s="59" t="s">
+      <c r="O4" s="48" t="s">
         <v>201</v>
       </c>
-      <c r="P4" s="59" t="s">
+      <c r="P4" s="48" t="s">
         <v>202</v>
       </c>
-      <c r="Q4" s="60" t="s">
+      <c r="Q4" s="49" t="s">
         <v>203</v>
       </c>
-      <c r="R4" s="59" t="s">
+      <c r="R4" s="48" t="s">
         <v>204</v>
       </c>
-      <c r="S4" s="59" t="s">
+      <c r="S4" s="48" t="s">
         <v>205</v>
       </c>
-      <c r="T4" s="60" t="s">
+      <c r="T4" s="49" t="s">
         <v>206</v>
       </c>
-      <c r="U4" s="59" t="s">
+      <c r="U4" s="48" t="s">
         <v>207</v>
       </c>
-      <c r="V4" s="61" t="s">
+      <c r="V4" s="50" t="s">
         <v>208</v>
       </c>
-      <c r="W4" s="59" t="s">
+      <c r="W4" s="48" t="s">
         <v>199</v>
       </c>
-      <c r="X4" s="60" t="s">
+      <c r="X4" s="49" t="s">
         <v>200</v>
       </c>
-      <c r="Y4" s="59" t="s">
+      <c r="Y4" s="48" t="s">
         <v>201</v>
       </c>
-      <c r="Z4" s="59" t="s">
+      <c r="Z4" s="48" t="s">
         <v>202</v>
       </c>
-      <c r="AA4" s="60" t="s">
+      <c r="AA4" s="49" t="s">
         <v>203</v>
       </c>
-      <c r="AB4" s="59" t="s">
+      <c r="AB4" s="48" t="s">
         <v>204</v>
       </c>
-      <c r="AC4" s="59" t="s">
+      <c r="AC4" s="48" t="s">
         <v>205</v>
       </c>
-      <c r="AD4" s="60" t="s">
+      <c r="AD4" s="49" t="s">
         <v>206</v>
       </c>
-      <c r="AE4" s="59" t="s">
+      <c r="AE4" s="48" t="s">
         <v>207</v>
       </c>
-      <c r="AF4" s="61" t="s">
+      <c r="AF4" s="50" t="s">
         <v>208</v>
       </c>
-      <c r="AG4" s="59" t="s">
+      <c r="AG4" s="48" t="s">
         <v>199</v>
       </c>
-      <c r="AH4" s="60" t="s">
+      <c r="AH4" s="49" t="s">
         <v>200</v>
       </c>
-      <c r="AI4" s="59" t="s">
+      <c r="AI4" s="48" t="s">
         <v>201</v>
       </c>
-      <c r="AJ4" s="59" t="s">
+      <c r="AJ4" s="48" t="s">
         <v>202</v>
       </c>
-      <c r="AK4" s="60" t="s">
+      <c r="AK4" s="49" t="s">
         <v>203</v>
       </c>
-      <c r="AL4" s="59" t="s">
+      <c r="AL4" s="48" t="s">
         <v>204</v>
       </c>
-      <c r="AM4" s="59" t="s">
+      <c r="AM4" s="48" t="s">
         <v>205</v>
       </c>
-      <c r="AN4" s="60" t="s">
+      <c r="AN4" s="49" t="s">
         <v>206</v>
       </c>
-      <c r="AO4" s="59" t="s">
+      <c r="AO4" s="48" t="s">
         <v>207</v>
       </c>
-      <c r="AP4" s="61" t="s">
+      <c r="AP4" s="50" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="5" spans="2:42" x14ac:dyDescent="0.35">
-      <c r="B5" s="43" t="s">
+      <c r="B5" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="C5" s="51"/>
+      <c r="C5" s="40"/>
       <c r="D5" s="35"/>
       <c r="E5" s="35"/>
       <c r="F5" s="35"/>
       <c r="G5" s="35"/>
       <c r="H5" s="35"/>
-      <c r="I5" s="46"/>
+      <c r="I5" s="39"/>
       <c r="J5" s="35"/>
       <c r="K5" s="35"/>
-      <c r="L5" s="56"/>
-      <c r="M5" s="51"/>
+      <c r="L5" s="45"/>
+      <c r="M5" s="40"/>
       <c r="N5" s="35"/>
       <c r="O5" s="35"/>
       <c r="P5" s="35"/>
       <c r="Q5" s="35"/>
       <c r="R5" s="35"/>
-      <c r="S5" s="46"/>
+      <c r="S5" s="39"/>
       <c r="T5" s="35"/>
       <c r="U5" s="35"/>
-      <c r="V5" s="56"/>
-      <c r="W5" s="51"/>
+      <c r="V5" s="45"/>
+      <c r="W5" s="40"/>
       <c r="X5" s="35"/>
       <c r="Y5" s="35"/>
       <c r="Z5" s="35"/>
       <c r="AA5" s="35"/>
       <c r="AB5" s="35"/>
-      <c r="AC5" s="46"/>
+      <c r="AC5" s="39"/>
       <c r="AD5" s="35"/>
       <c r="AE5" s="35"/>
-      <c r="AF5" s="56"/>
-      <c r="AG5" s="51"/>
+      <c r="AF5" s="45"/>
+      <c r="AG5" s="40"/>
       <c r="AH5" s="35"/>
       <c r="AI5" s="35"/>
       <c r="AJ5" s="35"/>
       <c r="AK5" s="35"/>
       <c r="AL5" s="35"/>
-      <c r="AM5" s="46"/>
+      <c r="AM5" s="39"/>
       <c r="AN5" s="35"/>
       <c r="AO5" s="35"/>
-      <c r="AP5" s="56"/>
+      <c r="AP5" s="45"/>
     </row>
     <row r="6" spans="2:42" x14ac:dyDescent="0.35">
-      <c r="B6" s="42" t="s">
+      <c r="B6" t="s">
         <v>49</v>
       </c>
-      <c r="C6" s="52">
+      <c r="C6" s="41">
         <v>-3959</v>
       </c>
       <c r="D6" s="20"/>
@@ -4527,7 +4744,7 @@
       <c r="I6" s="20"/>
       <c r="J6" s="20"/>
       <c r="K6" s="20"/>
-      <c r="L6" s="57"/>
+      <c r="L6" s="46"/>
       <c r="M6" s="21">
         <v>207.6</v>
       </c>
@@ -4539,7 +4756,7 @@
       <c r="S6" s="20"/>
       <c r="T6" s="20"/>
       <c r="U6" s="20"/>
-      <c r="V6" s="57"/>
+      <c r="V6" s="46"/>
       <c r="W6" s="21">
         <v>1525</v>
       </c>
@@ -4551,7 +4768,7 @@
       <c r="AC6" s="20"/>
       <c r="AD6" s="20"/>
       <c r="AE6" s="20"/>
-      <c r="AF6" s="57"/>
+      <c r="AF6" s="46"/>
       <c r="AG6" s="21">
         <v>62</v>
       </c>
@@ -4563,13 +4780,13 @@
       <c r="AM6" s="20"/>
       <c r="AN6" s="20"/>
       <c r="AO6" s="20"/>
-      <c r="AP6" s="57"/>
+      <c r="AP6" s="46"/>
     </row>
     <row r="7" spans="2:42" x14ac:dyDescent="0.35">
-      <c r="B7" s="42" t="s">
+      <c r="B7" t="s">
         <v>159</v>
       </c>
-      <c r="C7" s="53">
+      <c r="C7" s="42">
         <v>-0.85550000000000004</v>
       </c>
       <c r="D7" s="20"/>
@@ -4580,7 +4797,7 @@
       <c r="I7" s="20"/>
       <c r="J7" s="20"/>
       <c r="K7" s="20"/>
-      <c r="L7" s="57"/>
+      <c r="L7" s="46"/>
       <c r="M7" s="21">
         <v>197.2</v>
       </c>
@@ -4592,7 +4809,7 @@
       <c r="S7" s="20"/>
       <c r="T7" s="20"/>
       <c r="U7" s="20"/>
-      <c r="V7" s="57"/>
+      <c r="V7" s="46"/>
       <c r="W7" s="21">
         <v>1029</v>
       </c>
@@ -4604,7 +4821,7 @@
       <c r="AC7" s="20"/>
       <c r="AD7" s="20"/>
       <c r="AE7" s="20"/>
-      <c r="AF7" s="57"/>
+      <c r="AF7" s="46"/>
       <c r="AG7" s="21">
         <v>49</v>
       </c>
@@ -4616,13 +4833,13 @@
       <c r="AM7" s="20"/>
       <c r="AN7" s="20"/>
       <c r="AO7" s="20"/>
-      <c r="AP7" s="57"/>
+      <c r="AP7" s="46"/>
     </row>
     <row r="8" spans="2:42" x14ac:dyDescent="0.35">
-      <c r="B8" s="42" t="s">
+      <c r="B8" t="s">
         <v>50</v>
       </c>
-      <c r="C8" s="53">
+      <c r="C8" s="42">
         <v>12.52</v>
       </c>
       <c r="D8" s="20"/>
@@ -4633,7 +4850,7 @@
       <c r="I8" s="20"/>
       <c r="J8" s="20"/>
       <c r="K8" s="20"/>
-      <c r="L8" s="57"/>
+      <c r="L8" s="46"/>
       <c r="M8" s="21">
         <v>202.5</v>
       </c>
@@ -4645,7 +4862,7 @@
       <c r="S8" s="20"/>
       <c r="T8" s="20"/>
       <c r="U8" s="20"/>
-      <c r="V8" s="57"/>
+      <c r="V8" s="46"/>
       <c r="W8" s="21">
         <v>320</v>
       </c>
@@ -4657,7 +4874,7 @@
       <c r="AC8" s="20"/>
       <c r="AD8" s="20"/>
       <c r="AE8" s="20"/>
-      <c r="AF8" s="57"/>
+      <c r="AF8" s="46"/>
       <c r="AG8" s="21">
         <v>15</v>
       </c>
@@ -4669,11 +4886,10 @@
       <c r="AM8" s="20"/>
       <c r="AN8" s="20"/>
       <c r="AO8" s="20"/>
-      <c r="AP8" s="57"/>
+      <c r="AP8" s="46"/>
     </row>
     <row r="9" spans="2:42" x14ac:dyDescent="0.35">
-      <c r="B9" s="42"/>
-      <c r="C9" s="53"/>
+      <c r="C9" s="42"/>
       <c r="D9" s="20"/>
       <c r="E9" s="20"/>
       <c r="F9" s="20"/>
@@ -4682,7 +4898,7 @@
       <c r="I9" s="20"/>
       <c r="J9" s="20"/>
       <c r="K9" s="20"/>
-      <c r="L9" s="57"/>
+      <c r="L9" s="46"/>
       <c r="M9" s="21"/>
       <c r="N9" s="20"/>
       <c r="O9" s="20"/>
@@ -4692,7 +4908,7 @@
       <c r="S9" s="20"/>
       <c r="T9" s="20"/>
       <c r="U9" s="20"/>
-      <c r="V9" s="57"/>
+      <c r="V9" s="46"/>
       <c r="W9" s="20"/>
       <c r="X9" s="20"/>
       <c r="Y9" s="20"/>
@@ -4702,7 +4918,7 @@
       <c r="AC9" s="20"/>
       <c r="AD9" s="20"/>
       <c r="AE9" s="20"/>
-      <c r="AF9" s="57"/>
+      <c r="AF9" s="46"/>
       <c r="AG9" s="21"/>
       <c r="AH9" s="20"/>
       <c r="AI9" s="20"/>
@@ -4712,13 +4928,13 @@
       <c r="AM9" s="20"/>
       <c r="AN9" s="20"/>
       <c r="AO9" s="20"/>
-      <c r="AP9" s="57"/>
+      <c r="AP9" s="46"/>
     </row>
     <row r="10" spans="2:42" x14ac:dyDescent="0.35">
-      <c r="B10" s="43" t="s">
+      <c r="B10" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="C10" s="53"/>
+      <c r="C10" s="42"/>
       <c r="D10" s="35"/>
       <c r="E10" s="35"/>
       <c r="F10" s="35"/>
@@ -4727,7 +4943,7 @@
       <c r="I10" s="35"/>
       <c r="J10" s="35"/>
       <c r="K10" s="35"/>
-      <c r="L10" s="56"/>
+      <c r="L10" s="45"/>
       <c r="M10" s="21"/>
       <c r="N10" s="35"/>
       <c r="O10" s="35"/>
@@ -4737,7 +4953,7 @@
       <c r="S10" s="35"/>
       <c r="T10" s="35"/>
       <c r="U10" s="35"/>
-      <c r="V10" s="56"/>
+      <c r="V10" s="45"/>
       <c r="W10" s="20"/>
       <c r="X10" s="35"/>
       <c r="Y10" s="35"/>
@@ -4747,7 +4963,7 @@
       <c r="AC10" s="35"/>
       <c r="AD10" s="35"/>
       <c r="AE10" s="35"/>
-      <c r="AF10" s="56"/>
+      <c r="AF10" s="45"/>
       <c r="AG10" s="21"/>
       <c r="AH10" s="35"/>
       <c r="AI10" s="35"/>
@@ -4757,13 +4973,13 @@
       <c r="AM10" s="35"/>
       <c r="AN10" s="35"/>
       <c r="AO10" s="35"/>
-      <c r="AP10" s="56"/>
+      <c r="AP10" s="45"/>
     </row>
     <row r="11" spans="2:42" x14ac:dyDescent="0.35">
-      <c r="B11" s="42" t="s">
+      <c r="B11" t="s">
         <v>49</v>
       </c>
-      <c r="C11" s="52">
+      <c r="C11" s="41">
         <v>-3959</v>
       </c>
       <c r="D11" s="20"/>
@@ -4774,7 +4990,7 @@
       <c r="I11" s="20"/>
       <c r="J11" s="20"/>
       <c r="K11" s="20"/>
-      <c r="L11" s="57"/>
+      <c r="L11" s="46"/>
       <c r="M11" s="21">
         <v>207.6</v>
       </c>
@@ -4786,7 +5002,7 @@
       <c r="S11" s="20"/>
       <c r="T11" s="20"/>
       <c r="U11" s="20"/>
-      <c r="V11" s="57"/>
+      <c r="V11" s="46"/>
       <c r="W11" s="21">
         <v>1525</v>
       </c>
@@ -4798,7 +5014,7 @@
       <c r="AC11" s="20"/>
       <c r="AD11" s="20"/>
       <c r="AE11" s="20"/>
-      <c r="AF11" s="57"/>
+      <c r="AF11" s="46"/>
       <c r="AG11" s="21">
         <v>62</v>
       </c>
@@ -4810,13 +5026,13 @@
       <c r="AM11" s="20"/>
       <c r="AN11" s="20"/>
       <c r="AO11" s="20"/>
-      <c r="AP11" s="57"/>
+      <c r="AP11" s="46"/>
     </row>
     <row r="12" spans="2:42" x14ac:dyDescent="0.35">
-      <c r="B12" s="42" t="s">
+      <c r="B12" t="s">
         <v>159</v>
       </c>
-      <c r="C12" s="53"/>
+      <c r="C12" s="42"/>
       <c r="D12" s="20"/>
       <c r="E12" s="20"/>
       <c r="F12" s="20"/>
@@ -4825,8 +5041,8 @@
       <c r="I12" s="20"/>
       <c r="J12" s="20"/>
       <c r="K12" s="20"/>
-      <c r="L12" s="57"/>
-      <c r="M12" s="53"/>
+      <c r="L12" s="46"/>
+      <c r="M12" s="42"/>
       <c r="N12" s="20"/>
       <c r="O12" s="20"/>
       <c r="P12" s="20"/>
@@ -4835,8 +5051,8 @@
       <c r="S12" s="20"/>
       <c r="T12" s="20"/>
       <c r="U12" s="20"/>
-      <c r="V12" s="57"/>
-      <c r="W12" s="53"/>
+      <c r="V12" s="46"/>
+      <c r="W12" s="42"/>
       <c r="X12" s="20"/>
       <c r="Y12" s="20"/>
       <c r="Z12" s="20"/>
@@ -4845,8 +5061,8 @@
       <c r="AC12" s="20"/>
       <c r="AD12" s="20"/>
       <c r="AE12" s="20"/>
-      <c r="AF12" s="57"/>
-      <c r="AG12" s="53"/>
+      <c r="AF12" s="46"/>
+      <c r="AG12" s="42"/>
       <c r="AH12" s="20"/>
       <c r="AI12" s="20"/>
       <c r="AJ12" s="20"/>
@@ -4855,52 +5071,52 @@
       <c r="AM12" s="20"/>
       <c r="AN12" s="20"/>
       <c r="AO12" s="20"/>
-      <c r="AP12" s="57"/>
+      <c r="AP12" s="46"/>
     </row>
     <row r="13" spans="2:42" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B13" s="42" t="s">
+      <c r="B13" t="s">
         <v>50</v>
       </c>
-      <c r="C13" s="54"/>
-      <c r="D13" s="55"/>
-      <c r="E13" s="55"/>
-      <c r="F13" s="55"/>
-      <c r="G13" s="55"/>
-      <c r="H13" s="55"/>
-      <c r="I13" s="55"/>
-      <c r="J13" s="55"/>
-      <c r="K13" s="55"/>
-      <c r="L13" s="58"/>
-      <c r="M13" s="54"/>
-      <c r="N13" s="55"/>
-      <c r="O13" s="55"/>
-      <c r="P13" s="55"/>
-      <c r="Q13" s="55"/>
-      <c r="R13" s="55"/>
-      <c r="S13" s="55"/>
-      <c r="T13" s="55"/>
-      <c r="U13" s="55"/>
-      <c r="V13" s="58"/>
-      <c r="W13" s="54"/>
-      <c r="X13" s="55"/>
-      <c r="Y13" s="55"/>
-      <c r="Z13" s="55"/>
-      <c r="AA13" s="55"/>
-      <c r="AB13" s="55"/>
-      <c r="AC13" s="55"/>
-      <c r="AD13" s="55"/>
-      <c r="AE13" s="55"/>
-      <c r="AF13" s="58"/>
-      <c r="AG13" s="54"/>
-      <c r="AH13" s="55"/>
-      <c r="AI13" s="55"/>
-      <c r="AJ13" s="55"/>
-      <c r="AK13" s="55"/>
-      <c r="AL13" s="55"/>
-      <c r="AM13" s="55"/>
-      <c r="AN13" s="55"/>
-      <c r="AO13" s="55"/>
-      <c r="AP13" s="58"/>
+      <c r="C13" s="43"/>
+      <c r="D13" s="44"/>
+      <c r="E13" s="44"/>
+      <c r="F13" s="44"/>
+      <c r="G13" s="44"/>
+      <c r="H13" s="44"/>
+      <c r="I13" s="44"/>
+      <c r="J13" s="44"/>
+      <c r="K13" s="44"/>
+      <c r="L13" s="47"/>
+      <c r="M13" s="43"/>
+      <c r="N13" s="44"/>
+      <c r="O13" s="44"/>
+      <c r="P13" s="44"/>
+      <c r="Q13" s="44"/>
+      <c r="R13" s="44"/>
+      <c r="S13" s="44"/>
+      <c r="T13" s="44"/>
+      <c r="U13" s="44"/>
+      <c r="V13" s="47"/>
+      <c r="W13" s="43"/>
+      <c r="X13" s="44"/>
+      <c r="Y13" s="44"/>
+      <c r="Z13" s="44"/>
+      <c r="AA13" s="44"/>
+      <c r="AB13" s="44"/>
+      <c r="AC13" s="44"/>
+      <c r="AD13" s="44"/>
+      <c r="AE13" s="44"/>
+      <c r="AF13" s="47"/>
+      <c r="AG13" s="43"/>
+      <c r="AH13" s="44"/>
+      <c r="AI13" s="44"/>
+      <c r="AJ13" s="44"/>
+      <c r="AK13" s="44"/>
+      <c r="AL13" s="44"/>
+      <c r="AM13" s="44"/>
+      <c r="AN13" s="44"/>
+      <c r="AO13" s="44"/>
+      <c r="AP13" s="47"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -5367,7 +5583,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B4CCA38-C1E8-4E87-B1AA-966A071EE4EA}">
-  <dimension ref="B2:Y36"/>
+  <dimension ref="B2:U36"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="D46" sqref="D46"/>
@@ -5397,12 +5613,12 @@
     <col min="21" max="21" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:25" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B2" s="9" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="3" spans="2:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="22" t="s">
         <v>160</v>
       </c>
@@ -5419,7 +5635,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="2:25" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:21" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B4" s="35" t="s">
         <v>158</v>
       </c>
@@ -5428,7 +5644,7 @@
       <c r="E4" s="20"/>
       <c r="F4" s="21"/>
     </row>
-    <row r="5" spans="2:25" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B5" s="20" t="s">
         <v>49</v>
       </c>
@@ -5445,7 +5661,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="6" spans="2:25" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B6" s="20" t="s">
         <v>159</v>
       </c>
@@ -5462,7 +5678,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="2:25" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B7" s="20" t="s">
         <v>50</v>
       </c>
@@ -5479,25 +5695,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="2:25" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B8" s="20"/>
       <c r="C8" s="21"/>
       <c r="D8" s="21"/>
       <c r="E8" s="20"/>
       <c r="F8" s="21"/>
-      <c r="O8" s="44"/>
-      <c r="P8" s="44"/>
-      <c r="Q8" s="44"/>
-      <c r="R8" s="44"/>
-      <c r="S8" s="44"/>
-      <c r="T8" s="44"/>
-      <c r="U8" s="44"/>
-      <c r="V8" s="44"/>
-      <c r="W8" s="44"/>
-      <c r="X8" s="44"/>
-      <c r="Y8" s="44"/>
-    </row>
-    <row r="9" spans="2:25" x14ac:dyDescent="0.35">
+    </row>
+    <row r="9" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B9" s="35" t="s">
         <v>157</v>
       </c>
@@ -5505,19 +5710,8 @@
       <c r="D9" s="21"/>
       <c r="E9" s="20"/>
       <c r="F9" s="21"/>
-      <c r="O9" s="44"/>
-      <c r="P9" s="44"/>
-      <c r="Q9" s="44"/>
-      <c r="R9" s="44"/>
-      <c r="S9" s="44"/>
-      <c r="T9" s="44"/>
-      <c r="U9" s="44"/>
-      <c r="V9" s="44"/>
-      <c r="W9" s="44"/>
-      <c r="X9" s="44"/>
-      <c r="Y9" s="44"/>
-    </row>
-    <row r="10" spans="2:25" x14ac:dyDescent="0.35">
+    </row>
+    <row r="10" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B10" s="20" t="s">
         <v>49</v>
       </c>
@@ -5533,19 +5727,8 @@
       <c r="F10" s="21">
         <v>62</v>
       </c>
-      <c r="O10" s="44"/>
-      <c r="P10" s="44"/>
-      <c r="Q10" s="44"/>
-      <c r="R10" s="44"/>
-      <c r="S10" s="44"/>
-      <c r="T10" s="44"/>
-      <c r="U10" s="44"/>
-      <c r="V10" s="44"/>
-      <c r="W10" s="44"/>
-      <c r="X10" s="44"/>
-      <c r="Y10" s="44"/>
-    </row>
-    <row r="11" spans="2:25" x14ac:dyDescent="0.35">
+    </row>
+    <row r="11" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B11" s="20" t="s">
         <v>159</v>
       </c>
@@ -5553,19 +5736,13 @@
       <c r="D11" s="20"/>
       <c r="E11" s="21"/>
       <c r="F11" s="21"/>
-      <c r="O11" s="44"/>
-      <c r="P11" s="44"/>
-      <c r="Q11" s="45"/>
-      <c r="R11" s="45"/>
-      <c r="S11" s="45"/>
-      <c r="T11" s="45"/>
-      <c r="U11" s="45"/>
-      <c r="V11" s="44"/>
-      <c r="W11" s="44"/>
-      <c r="X11" s="44"/>
-      <c r="Y11" s="44"/>
-    </row>
-    <row r="12" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="Q11" s="9"/>
+      <c r="R11" s="9"/>
+      <c r="S11" s="9"/>
+      <c r="T11" s="9"/>
+      <c r="U11" s="9"/>
+    </row>
+    <row r="12" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B12" s="20" t="s">
         <v>50</v>
       </c>
@@ -5573,61 +5750,14 @@
       <c r="D12" s="21"/>
       <c r="E12" s="21"/>
       <c r="F12" s="21"/>
-      <c r="O12" s="44"/>
-      <c r="P12" s="44"/>
-      <c r="Q12" s="45"/>
-      <c r="R12" s="44"/>
-      <c r="S12" s="44"/>
-      <c r="T12" s="44"/>
-      <c r="U12" s="44"/>
-      <c r="V12" s="44"/>
-      <c r="W12" s="44"/>
-      <c r="X12" s="44"/>
-      <c r="Y12" s="44"/>
-    </row>
-    <row r="13" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="O13" s="44"/>
-      <c r="P13" s="44"/>
-      <c r="Q13" s="44"/>
-      <c r="R13" s="44"/>
-      <c r="S13" s="44"/>
-      <c r="T13" s="44"/>
-      <c r="U13" s="44"/>
-      <c r="V13" s="44"/>
-      <c r="W13" s="44"/>
-      <c r="X13" s="44"/>
-      <c r="Y13" s="44"/>
-    </row>
-    <row r="14" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="O14" s="44"/>
-      <c r="P14" s="44"/>
-      <c r="Q14" s="44"/>
-      <c r="R14" s="44"/>
-      <c r="S14" s="44"/>
-      <c r="T14" s="44"/>
-      <c r="U14" s="44"/>
-      <c r="V14" s="44"/>
-      <c r="W14" s="44"/>
-      <c r="X14" s="44"/>
-      <c r="Y14" s="44"/>
-    </row>
-    <row r="15" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="Q12" s="9"/>
+    </row>
+    <row r="15" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B15" s="9" t="s">
         <v>196</v>
       </c>
-      <c r="O15" s="44"/>
-      <c r="P15" s="44"/>
-      <c r="Q15" s="44"/>
-      <c r="R15" s="44"/>
-      <c r="S15" s="44"/>
-      <c r="T15" s="44"/>
-      <c r="U15" s="44"/>
-      <c r="V15" s="44"/>
-      <c r="W15" s="44"/>
-      <c r="X15" s="44"/>
-      <c r="Y15" s="44"/>
-    </row>
-    <row r="16" spans="2:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="16" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B16" s="22" t="s">
         <v>122</v>
       </c>
@@ -5652,19 +5782,9 @@
       <c r="I16" s="23" t="s">
         <v>136</v>
       </c>
-      <c r="O16" s="44"/>
-      <c r="P16" s="44"/>
-      <c r="Q16" s="45"/>
-      <c r="R16" s="44"/>
-      <c r="S16" s="44"/>
-      <c r="T16" s="44"/>
-      <c r="U16" s="44"/>
-      <c r="V16" s="44"/>
-      <c r="W16" s="44"/>
-      <c r="X16" s="44"/>
-      <c r="Y16" s="44"/>
-    </row>
-    <row r="17" spans="2:25" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="Q16" s="9"/>
+    </row>
+    <row r="17" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B17" s="35" t="s">
         <v>126</v>
       </c>
@@ -5675,19 +5795,8 @@
       <c r="G17" s="21"/>
       <c r="H17" s="21"/>
       <c r="I17" s="21"/>
-      <c r="O17" s="44"/>
-      <c r="P17" s="44"/>
-      <c r="Q17" s="44"/>
-      <c r="R17" s="44"/>
-      <c r="S17" s="44"/>
-      <c r="T17" s="44"/>
-      <c r="U17" s="44"/>
-      <c r="V17" s="44"/>
-      <c r="W17" s="44"/>
-      <c r="X17" s="44"/>
-      <c r="Y17" s="44"/>
-    </row>
-    <row r="18" spans="2:25" x14ac:dyDescent="0.35">
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B18" s="20" t="s">
         <v>123</v>
       </c>
@@ -5712,19 +5821,8 @@
       <c r="I18" s="21" t="s">
         <v>183</v>
       </c>
-      <c r="O18" s="44"/>
-      <c r="P18" s="44"/>
-      <c r="Q18" s="44"/>
-      <c r="R18" s="44"/>
-      <c r="S18" s="44"/>
-      <c r="T18" s="44"/>
-      <c r="U18" s="44"/>
-      <c r="V18" s="44"/>
-      <c r="W18" s="44"/>
-      <c r="X18" s="44"/>
-      <c r="Y18" s="44"/>
-    </row>
-    <row r="19" spans="2:25" x14ac:dyDescent="0.35">
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B19" s="20" t="s">
         <v>124</v>
       </c>
@@ -5749,19 +5847,8 @@
       <c r="I19" s="21" t="s">
         <v>184</v>
       </c>
-      <c r="O19" s="44"/>
-      <c r="P19" s="44"/>
-      <c r="Q19" s="44"/>
-      <c r="R19" s="44"/>
-      <c r="S19" s="44"/>
-      <c r="T19" s="44"/>
-      <c r="U19" s="44"/>
-      <c r="V19" s="44"/>
-      <c r="W19" s="44"/>
-      <c r="X19" s="44"/>
-      <c r="Y19" s="44"/>
-    </row>
-    <row r="20" spans="2:25" x14ac:dyDescent="0.35">
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
         <v>125</v>
       </c>
@@ -5786,19 +5873,8 @@
       <c r="I20" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="O20" s="44"/>
-      <c r="P20" s="44"/>
-      <c r="Q20" s="44"/>
-      <c r="R20" s="44"/>
-      <c r="S20" s="44"/>
-      <c r="T20" s="44"/>
-      <c r="U20" s="44"/>
-      <c r="V20" s="44"/>
-      <c r="W20" s="44"/>
-      <c r="X20" s="44"/>
-      <c r="Y20" s="44"/>
-    </row>
-    <row r="21" spans="2:25" x14ac:dyDescent="0.35">
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B21" s="20"/>
       <c r="C21" s="21"/>
       <c r="D21" s="21"/>
@@ -5807,19 +5883,8 @@
       <c r="G21" s="21"/>
       <c r="H21" s="21"/>
       <c r="I21" s="21"/>
-      <c r="O21" s="44"/>
-      <c r="P21" s="44"/>
-      <c r="Q21" s="44"/>
-      <c r="R21" s="44"/>
-      <c r="S21" s="44"/>
-      <c r="T21" s="44"/>
-      <c r="U21" s="44"/>
-      <c r="V21" s="44"/>
-      <c r="W21" s="44"/>
-      <c r="X21" s="44"/>
-      <c r="Y21" s="44"/>
-    </row>
-    <row r="22" spans="2:25" x14ac:dyDescent="0.35">
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B22" s="35" t="s">
         <v>127</v>
       </c>
@@ -5830,19 +5895,8 @@
       <c r="G22" s="21"/>
       <c r="H22" s="21"/>
       <c r="I22" s="21"/>
-      <c r="O22" s="44"/>
-      <c r="P22" s="44"/>
-      <c r="Q22" s="44"/>
-      <c r="R22" s="44"/>
-      <c r="S22" s="44"/>
-      <c r="T22" s="44"/>
-      <c r="U22" s="44"/>
-      <c r="V22" s="44"/>
-      <c r="W22" s="44"/>
-      <c r="X22" s="44"/>
-      <c r="Y22" s="44"/>
-    </row>
-    <row r="23" spans="2:25" x14ac:dyDescent="0.35">
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B23" s="20" t="s">
         <v>123</v>
       </c>
@@ -5867,19 +5921,8 @@
       <c r="I23" s="21" t="s">
         <v>182</v>
       </c>
-      <c r="O23" s="44"/>
-      <c r="P23" s="44"/>
-      <c r="Q23" s="44"/>
-      <c r="R23" s="44"/>
-      <c r="S23" s="44"/>
-      <c r="T23" s="44"/>
-      <c r="U23" s="44"/>
-      <c r="V23" s="44"/>
-      <c r="W23" s="44"/>
-      <c r="X23" s="44"/>
-      <c r="Y23" s="44"/>
-    </row>
-    <row r="24" spans="2:25" x14ac:dyDescent="0.35">
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B24" s="20" t="s">
         <v>124</v>
       </c>
@@ -5905,7 +5948,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="25" spans="2:25" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
         <v>125</v>
       </c>
@@ -5931,12 +5974,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="28" spans="2:25" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B28" s="9" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="29" spans="2:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B29" s="22" t="s">
         <v>122</v>
       </c>
@@ -5953,7 +5996,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="30" spans="2:25" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B30" s="35" t="s">
         <v>126</v>
       </c>
@@ -5961,7 +6004,7 @@
       <c r="E30" s="21"/>
       <c r="F30" s="21"/>
     </row>
-    <row r="31" spans="2:25" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B31" s="20" t="s">
         <v>123</v>
       </c>
@@ -5978,7 +6021,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="32" spans="2:25" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B32" s="20" t="s">
         <v>124</v>
       </c>

</xml_diff>